<commit_message>
changed map route colors and text for light markers
</commit_message>
<xml_diff>
--- a/archived_versions/vrp_results_tracker_02.xlsx
+++ b/archived_versions/vrp_results_tracker_02.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zzzlib\PycharmProjects\wilib_vrp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdrex\PycharmProjects\wilib_vrp\archived_versions\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF76044D-8C8A-4E62-BA76-20BE28B26241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test_model_set" sheetId="4" r:id="rId1"/>
     <sheet name="reduced_model_set_copy" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="141">
   <si>
     <t>shift</t>
   </si>
@@ -397,12 +399,72 @@
   </si>
   <si>
     <t>t1005</t>
+  </si>
+  <si>
+    <t>n_vehicles</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>duration</t>
+  </si>
+  <si>
+    <t>8 hour</t>
+  </si>
+  <si>
+    <t>10 hour</t>
+  </si>
+  <si>
+    <t>ideal 1</t>
+  </si>
+  <si>
+    <t>ideal 2</t>
+  </si>
+  <si>
+    <t>ideal 3</t>
+  </si>
+  <si>
+    <t>ideal 4</t>
+  </si>
+  <si>
+    <t>ideal 5</t>
+  </si>
+  <si>
+    <t>ideal 6</t>
+  </si>
+  <si>
+    <t>ideal 7</t>
+  </si>
+  <si>
+    <t>starter 7</t>
+  </si>
+  <si>
+    <t>starter 8</t>
+  </si>
+  <si>
+    <t>starter 1</t>
+  </si>
+  <si>
+    <t>starter 2</t>
+  </si>
+  <si>
+    <t>starter 3</t>
+  </si>
+  <si>
+    <t>starter 4</t>
+  </si>
+  <si>
+    <t>starter 5</t>
+  </si>
+  <si>
+    <t>starter 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -536,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -566,6 +628,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,21 +958,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" customWidth="1"/>
-    <col min="2" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="10.453125" customWidth="1"/>
+    <col min="2" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>70</v>
       </c>
@@ -918,7 +986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>71</v>
       </c>
@@ -932,7 +1000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>72</v>
       </c>
@@ -946,7 +1014,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>73</v>
       </c>
@@ -960,7 +1028,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>74</v>
       </c>
@@ -974,7 +1042,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>75</v>
       </c>
@@ -988,7 +1056,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>76</v>
       </c>
@@ -1002,7 +1070,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>77</v>
       </c>
@@ -1016,7 +1084,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>78</v>
       </c>
@@ -1030,7 +1098,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>79</v>
       </c>
@@ -1044,7 +1112,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>80</v>
       </c>
@@ -1058,7 +1126,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>81</v>
       </c>
@@ -1069,7 +1137,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>82</v>
       </c>
@@ -1080,7 +1148,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>83</v>
       </c>
@@ -1091,7 +1159,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>84</v>
       </c>
@@ -1102,7 +1170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>85</v>
       </c>
@@ -1113,7 +1181,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>86</v>
       </c>
@@ -1127,7 +1195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>87</v>
       </c>
@@ -1141,7 +1209,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>88</v>
       </c>
@@ -1155,7 +1223,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>89</v>
       </c>
@@ -1169,7 +1237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>90</v>
       </c>
@@ -1183,7 +1251,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>91</v>
       </c>
@@ -1197,7 +1265,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>92</v>
       </c>
@@ -1211,7 +1279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>93</v>
       </c>
@@ -1225,7 +1293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>94</v>
       </c>
@@ -1239,7 +1307,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>95</v>
       </c>
@@ -1253,7 +1321,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>96</v>
       </c>
@@ -1267,7 +1335,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>97</v>
       </c>
@@ -1281,7 +1349,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>98</v>
       </c>
@@ -1295,7 +1363,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>99</v>
       </c>
@@ -1309,7 +1377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>100</v>
       </c>
@@ -1323,7 +1391,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>101</v>
       </c>
@@ -1337,7 +1405,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>102</v>
       </c>
@@ -1351,7 +1419,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>103</v>
       </c>
@@ -1365,7 +1433,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>104</v>
       </c>
@@ -1379,7 +1447,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>105</v>
       </c>
@@ -1393,7 +1461,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>106</v>
       </c>
@@ -1407,7 +1475,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>107</v>
       </c>
@@ -1421,7 +1489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>108</v>
       </c>
@@ -1435,7 +1503,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>109</v>
       </c>
@@ -1449,7 +1517,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>110</v>
       </c>
@@ -1463,7 +1531,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>111</v>
       </c>
@@ -1477,7 +1545,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>112</v>
       </c>
@@ -1491,7 +1559,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>113</v>
       </c>
@@ -1505,7 +1573,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>114</v>
       </c>
@@ -1519,7 +1587,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>115</v>
       </c>
@@ -1533,7 +1601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>116</v>
       </c>
@@ -1547,7 +1615,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>117</v>
       </c>
@@ -1561,7 +1629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>118</v>
       </c>
@@ -1575,7 +1643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>119</v>
       </c>
@@ -1589,7 +1657,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>120</v>
       </c>
@@ -1610,22 +1678,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
-    <col min="2" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="20" width="10.5703125" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" style="1" customWidth="1"/>
+    <col min="2" max="5" width="15.54296875" customWidth="1"/>
+    <col min="6" max="20" width="10.54296875" customWidth="1"/>
+    <col min="21" max="21" width="16.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>70</v>
       </c>
@@ -1690,7 +1758,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>38</v>
       </c>
@@ -1755,7 +1823,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>39</v>
       </c>
@@ -1820,7 +1888,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>40</v>
       </c>
@@ -1885,7 +1953,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>41</v>
       </c>
@@ -1950,7 +2018,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
@@ -2015,7 +2083,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>43</v>
       </c>
@@ -2080,7 +2148,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>44</v>
       </c>
@@ -2145,7 +2213,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>45</v>
       </c>
@@ -2210,7 +2278,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -2275,7 +2343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>47</v>
       </c>
@@ -2340,7 +2408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>48</v>
       </c>
@@ -2405,7 +2473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>49</v>
       </c>
@@ -2470,7 +2538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>50</v>
       </c>
@@ -2535,7 +2603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>51</v>
       </c>
@@ -2600,7 +2668,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>52</v>
       </c>
@@ -2665,7 +2733,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>53</v>
       </c>
@@ -2730,7 +2798,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>54</v>
       </c>
@@ -2795,7 +2863,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>55</v>
       </c>
@@ -2860,7 +2928,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>56</v>
       </c>
@@ -2925,7 +2993,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>57</v>
       </c>
@@ -2990,7 +3058,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>58</v>
       </c>
@@ -3055,7 +3123,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>59</v>
       </c>
@@ -3120,7 +3188,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>60</v>
       </c>
@@ -3185,7 +3253,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>61</v>
       </c>
@@ -3250,7 +3318,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>62</v>
       </c>
@@ -3313,7 +3381,7 @@
       </c>
       <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>63</v>
       </c>
@@ -3376,7 +3444,7 @@
       </c>
       <c r="U27" s="1"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>64</v>
       </c>
@@ -3439,7 +3507,7 @@
       </c>
       <c r="U28" s="1"/>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>65</v>
       </c>
@@ -3502,7 +3570,7 @@
       </c>
       <c r="U29" s="1"/>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>66</v>
       </c>
@@ -3565,7 +3633,7 @@
       </c>
       <c r="U30" s="1"/>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>67</v>
       </c>
@@ -3628,7 +3696,7 @@
       </c>
       <c r="U31" s="1"/>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>68</v>
       </c>
@@ -3691,7 +3759,7 @@
       </c>
       <c r="U32" s="1"/>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>69</v>
       </c>
@@ -3764,4 +3832,2960 @@
     <ignoredError sqref="A2:A25 A26:A33" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D8E285-8EFA-4B6B-8917-C1FF6A22409E}">
+  <dimension ref="A1:O56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46:G49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="I1" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="6"/>
+      <c r="B2" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O2" s="27"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6">
+        <v>9</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2177.8000000000002</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="6">
+        <f>68*60+22</f>
+        <v>4102</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="6">
+        <v>6</v>
+      </c>
+      <c r="K4" s="6">
+        <v>4</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1335.41</v>
+      </c>
+      <c r="M4" s="11">
+        <v>1063.6600000000001</v>
+      </c>
+      <c r="N4" s="6">
+        <f>43*60+6</f>
+        <v>2586</v>
+      </c>
+      <c r="O4" s="6">
+        <f>35*60+35</f>
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6">
+        <v>7</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2211.38</v>
+      </c>
+      <c r="E5" s="11">
+        <v>1765.12</v>
+      </c>
+      <c r="F5" s="6">
+        <f>69*60+46</f>
+        <v>4186</v>
+      </c>
+      <c r="G5" s="6">
+        <f>59*60+12</f>
+        <v>3552</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="6">
+        <v>6</v>
+      </c>
+      <c r="K5" s="6">
+        <v>5</v>
+      </c>
+      <c r="L5" s="6">
+        <v>1360.19</v>
+      </c>
+      <c r="M5" s="11">
+        <v>1169.03</v>
+      </c>
+      <c r="N5" s="6">
+        <f>43*60+32</f>
+        <v>2612</v>
+      </c>
+      <c r="O5" s="6">
+        <f>38*60+4</f>
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="6">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6">
+        <v>7</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2197.42</v>
+      </c>
+      <c r="E6" s="11">
+        <v>1841.94</v>
+      </c>
+      <c r="F6" s="6">
+        <f>69*60+6</f>
+        <v>4146</v>
+      </c>
+      <c r="G6" s="6">
+        <f>61*60+11</f>
+        <v>3671</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="6">
+        <v>6</v>
+      </c>
+      <c r="K6" s="6">
+        <v>6</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1362.96</v>
+      </c>
+      <c r="M6" s="11">
+        <v>1327.72</v>
+      </c>
+      <c r="N6" s="6">
+        <f>43*60+33</f>
+        <v>2613</v>
+      </c>
+      <c r="O6" s="6">
+        <f>42*60+38</f>
+        <v>2558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="9">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9">
+        <v>8</v>
+      </c>
+      <c r="D7" s="9">
+        <v>2373.54</v>
+      </c>
+      <c r="E7" s="9">
+        <v>2033.75</v>
+      </c>
+      <c r="F7" s="9">
+        <f>71*60+36</f>
+        <v>4296</v>
+      </c>
+      <c r="G7" s="9">
+        <f>65*60+35</f>
+        <v>3935</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" s="9">
+        <v>6</v>
+      </c>
+      <c r="K7" s="9">
+        <v>4</v>
+      </c>
+      <c r="L7" s="9">
+        <v>1279.94</v>
+      </c>
+      <c r="M7" s="9">
+        <v>1143.44</v>
+      </c>
+      <c r="N7" s="9">
+        <f>41*60+18</f>
+        <v>2478</v>
+      </c>
+      <c r="O7" s="9">
+        <f>36*60+58</f>
+        <v>2218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="I8" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="J8" s="27"/>
+      <c r="K8" s="27"/>
+      <c r="L8" s="27"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="27"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="6"/>
+      <c r="B9" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="27"/>
+      <c r="F9" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="27"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" s="27"/>
+      <c r="L9" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M9" s="27"/>
+      <c r="N9" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O9" s="27"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6">
+        <v>5</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1444.82</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="6">
+        <f>47*60+46</f>
+        <v>2866</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="6">
+        <v>5</v>
+      </c>
+      <c r="K11" s="6">
+        <v>3</v>
+      </c>
+      <c r="L11" s="6">
+        <v>1105.77</v>
+      </c>
+      <c r="M11" s="11">
+        <v>795.08</v>
+      </c>
+      <c r="N11" s="6">
+        <f>60*35+9</f>
+        <v>2109</v>
+      </c>
+      <c r="O11" s="6">
+        <f>28*60+57</f>
+        <v>1737</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="6">
+        <v>8</v>
+      </c>
+      <c r="C12" s="6">
+        <v>6</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1825.59</v>
+      </c>
+      <c r="E12" s="11">
+        <v>1485.13</v>
+      </c>
+      <c r="F12" s="6">
+        <f>58*60+18</f>
+        <v>3498</v>
+      </c>
+      <c r="G12" s="6">
+        <f>49*60+30</f>
+        <v>2970</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="6">
+        <v>5</v>
+      </c>
+      <c r="K12" s="6">
+        <v>4</v>
+      </c>
+      <c r="L12" s="6">
+        <v>1024.1400000000001</v>
+      </c>
+      <c r="M12" s="11">
+        <v>980.51</v>
+      </c>
+      <c r="N12" s="6">
+        <f>34*60+20</f>
+        <v>2060</v>
+      </c>
+      <c r="O12" s="6">
+        <f>33*60+30</f>
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="6">
+        <v>9</v>
+      </c>
+      <c r="C13" s="6">
+        <v>6</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2003.37</v>
+      </c>
+      <c r="E13" s="6">
+        <v>1468.5</v>
+      </c>
+      <c r="F13" s="6">
+        <f>62*60+28</f>
+        <v>3748</v>
+      </c>
+      <c r="G13" s="6">
+        <f>48*60+20</f>
+        <v>2900</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="6">
+        <v>5</v>
+      </c>
+      <c r="K13" s="6">
+        <v>4</v>
+      </c>
+      <c r="L13" s="6">
+        <v>1004.07</v>
+      </c>
+      <c r="M13" s="11">
+        <v>906.65</v>
+      </c>
+      <c r="N13" s="6">
+        <f>34*60+7</f>
+        <v>2047</v>
+      </c>
+      <c r="O13" s="6">
+        <f>31*60+42</f>
+        <v>1902</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="9">
+        <v>8</v>
+      </c>
+      <c r="C14" s="9">
+        <v>6</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1750.27</v>
+      </c>
+      <c r="E14" s="9">
+        <v>1522.08</v>
+      </c>
+      <c r="F14" s="9">
+        <f>56*60+9</f>
+        <v>3369</v>
+      </c>
+      <c r="G14" s="9">
+        <f>49*60+46</f>
+        <v>2986</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="9">
+        <v>5</v>
+      </c>
+      <c r="K14" s="9">
+        <v>4</v>
+      </c>
+      <c r="L14" s="9">
+        <v>1048.51</v>
+      </c>
+      <c r="M14" s="9">
+        <v>1036.79</v>
+      </c>
+      <c r="N14" s="9">
+        <f>34*60 + 34</f>
+        <v>2074</v>
+      </c>
+      <c r="O14" s="9">
+        <f>34*60+25</f>
+        <v>2065</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="I15" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="J15" s="27"/>
+      <c r="K15" s="27"/>
+      <c r="L15" s="27"/>
+      <c r="M15" s="27"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="27"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" s="6"/>
+      <c r="B16" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O16" s="27"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="6">
+        <v>5</v>
+      </c>
+      <c r="C18" s="6">
+        <v>4</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1104.1500000000001</v>
+      </c>
+      <c r="E18" s="11">
+        <v>985.32</v>
+      </c>
+      <c r="F18" s="6">
+        <f>38*60+47</f>
+        <v>2327</v>
+      </c>
+      <c r="G18" s="6">
+        <f>35*60+35</f>
+        <v>2135</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="6">
+        <v>3</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="6">
+        <v>848.67</v>
+      </c>
+      <c r="N18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="6">
+        <f>27*60+55</f>
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="6">
+        <v>7</v>
+      </c>
+      <c r="C19" s="6">
+        <v>5</v>
+      </c>
+      <c r="D19" s="6">
+        <v>1318.36</v>
+      </c>
+      <c r="E19" s="11">
+        <v>1127.8699999999999</v>
+      </c>
+      <c r="F19" s="6">
+        <f>43*60+0</f>
+        <v>2580</v>
+      </c>
+      <c r="G19" s="6">
+        <f>38*60+45</f>
+        <v>2325</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="6">
+        <v>5</v>
+      </c>
+      <c r="K19" s="6">
+        <v>3</v>
+      </c>
+      <c r="L19" s="6">
+        <v>1045.72</v>
+      </c>
+      <c r="M19" s="11">
+        <v>780.37</v>
+      </c>
+      <c r="N19" s="6">
+        <f>33*60+54</f>
+        <v>2034</v>
+      </c>
+      <c r="O19" s="6">
+        <f>26*60+7</f>
+        <v>1567</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="6">
+        <v>7</v>
+      </c>
+      <c r="C20" s="6">
+        <v>6</v>
+      </c>
+      <c r="D20" s="6">
+        <v>1304.95</v>
+      </c>
+      <c r="E20" s="11">
+        <v>1283.95</v>
+      </c>
+      <c r="F20" s="6">
+        <f>42*60+14</f>
+        <v>2534</v>
+      </c>
+      <c r="G20" s="6">
+        <f>42*60+41</f>
+        <v>2561</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J20" s="6">
+        <v>5</v>
+      </c>
+      <c r="K20" s="6">
+        <v>4</v>
+      </c>
+      <c r="L20" s="6">
+        <v>1049.17</v>
+      </c>
+      <c r="M20" s="11">
+        <v>993.83</v>
+      </c>
+      <c r="N20" s="6">
+        <f>33*60+53</f>
+        <v>2033</v>
+      </c>
+      <c r="O20" s="6">
+        <f>32*60+8</f>
+        <v>1928</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B21" s="9">
+        <v>7</v>
+      </c>
+      <c r="C21" s="9">
+        <v>5</v>
+      </c>
+      <c r="D21" s="9">
+        <v>1412.54</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1156.9000000000001</v>
+      </c>
+      <c r="F21" s="9">
+        <f>45*60+36</f>
+        <v>2736</v>
+      </c>
+      <c r="G21" s="9">
+        <f>39*60+49</f>
+        <v>2389</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J21" s="9">
+        <v>5</v>
+      </c>
+      <c r="K21" s="9">
+        <v>4</v>
+      </c>
+      <c r="L21" s="9">
+        <v>1018.05</v>
+      </c>
+      <c r="M21" s="9">
+        <v>906.93</v>
+      </c>
+      <c r="N21" s="9">
+        <f>32*60+28</f>
+        <v>1948</v>
+      </c>
+      <c r="O21" s="9">
+        <f>30*60+3</f>
+        <v>1803</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A22" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="I22" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A23" s="6"/>
+      <c r="B23" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="27"/>
+      <c r="D23" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="27"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M23" s="27"/>
+      <c r="N23" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O23" s="27"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O24" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="6">
+        <v>5</v>
+      </c>
+      <c r="C25" s="6">
+        <v>4</v>
+      </c>
+      <c r="D25" s="6">
+        <v>941.06</v>
+      </c>
+      <c r="E25" s="11">
+        <v>881.17</v>
+      </c>
+      <c r="F25" s="6">
+        <f>33*60+2</f>
+        <v>1982</v>
+      </c>
+      <c r="G25" s="6">
+        <f>31*60+56</f>
+        <v>1916</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" s="6">
+        <v>5</v>
+      </c>
+      <c r="K25" s="6">
+        <v>4</v>
+      </c>
+      <c r="L25" s="6">
+        <v>1104.1500000000001</v>
+      </c>
+      <c r="M25" s="11">
+        <v>985.32</v>
+      </c>
+      <c r="N25" s="6">
+        <f>38*60+47</f>
+        <v>2327</v>
+      </c>
+      <c r="O25" s="6">
+        <f>35*60+35</f>
+        <v>2135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6</v>
+      </c>
+      <c r="C26" s="6">
+        <v>4</v>
+      </c>
+      <c r="D26" s="6">
+        <v>999.83</v>
+      </c>
+      <c r="E26" s="11">
+        <v>882.19</v>
+      </c>
+      <c r="F26" s="6">
+        <f>32*60+22</f>
+        <v>1942</v>
+      </c>
+      <c r="G26" s="6">
+        <f>32*60+15</f>
+        <v>1935</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J26" s="6">
+        <v>7</v>
+      </c>
+      <c r="K26" s="6">
+        <v>5</v>
+      </c>
+      <c r="L26" s="6">
+        <v>1329.89</v>
+      </c>
+      <c r="M26" s="11">
+        <v>1127.8699999999999</v>
+      </c>
+      <c r="N26" s="6">
+        <f>42*60+45</f>
+        <v>2565</v>
+      </c>
+      <c r="O26" s="6">
+        <f>38*60+45</f>
+        <v>2325</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="6">
+        <v>5</v>
+      </c>
+      <c r="C27" s="6">
+        <v>4</v>
+      </c>
+      <c r="D27" s="6">
+        <v>929.49</v>
+      </c>
+      <c r="E27" s="6">
+        <v>972.51</v>
+      </c>
+      <c r="F27" s="6">
+        <f>33*60+20</f>
+        <v>2000</v>
+      </c>
+      <c r="G27" s="6">
+        <f>33*60+15</f>
+        <v>1995</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J27" s="6">
+        <v>7</v>
+      </c>
+      <c r="K27" s="6">
+        <v>6</v>
+      </c>
+      <c r="L27" s="6">
+        <v>1304.95</v>
+      </c>
+      <c r="M27" s="11">
+        <v>1283.95</v>
+      </c>
+      <c r="N27" s="6">
+        <f>42*60+14</f>
+        <v>2534</v>
+      </c>
+      <c r="O27" s="6">
+        <f>42*60+41</f>
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="9">
+        <v>5</v>
+      </c>
+      <c r="C28" s="9">
+        <v>4</v>
+      </c>
+      <c r="D28" s="9">
+        <v>959.92</v>
+      </c>
+      <c r="E28" s="9">
+        <v>951.6</v>
+      </c>
+      <c r="F28" s="9">
+        <f>33*60+32</f>
+        <v>2012</v>
+      </c>
+      <c r="G28" s="9">
+        <f>34*60+0</f>
+        <v>2040</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="9">
+        <v>7</v>
+      </c>
+      <c r="K28" s="9">
+        <v>5</v>
+      </c>
+      <c r="L28" s="9">
+        <v>1412.54</v>
+      </c>
+      <c r="M28" s="9">
+        <v>1120.31</v>
+      </c>
+      <c r="N28" s="9">
+        <f>45*60+36</f>
+        <v>2736</v>
+      </c>
+      <c r="O28" s="9">
+        <f>38*60+55</f>
+        <v>2335</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="I29" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" s="6"/>
+      <c r="B30" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E30" s="27"/>
+      <c r="F30" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="27"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M30" s="27"/>
+      <c r="N30" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O30" s="27"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="6">
+        <v>6</v>
+      </c>
+      <c r="C32" s="6">
+        <v>4</v>
+      </c>
+      <c r="D32" s="6">
+        <v>1114.44</v>
+      </c>
+      <c r="E32" s="11">
+        <v>1007.94</v>
+      </c>
+      <c r="F32" s="6">
+        <f>42*60+1</f>
+        <v>2521</v>
+      </c>
+      <c r="G32" s="6">
+        <f>39*60+13</f>
+        <v>2353</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="6">
+        <v>4</v>
+      </c>
+      <c r="K32" s="6">
+        <v>3</v>
+      </c>
+      <c r="L32" s="6">
+        <v>714.67</v>
+      </c>
+      <c r="M32" s="11">
+        <v>773.89</v>
+      </c>
+      <c r="N32" s="6">
+        <f>25*60 +53</f>
+        <v>1553</v>
+      </c>
+      <c r="O32" s="6">
+        <f>26*60+47</f>
+        <v>1607</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="6">
+        <v>6</v>
+      </c>
+      <c r="C33" s="6">
+        <v>5</v>
+      </c>
+      <c r="D33" s="6">
+        <v>1113.44</v>
+      </c>
+      <c r="E33" s="11">
+        <v>1009.44</v>
+      </c>
+      <c r="F33" s="6">
+        <f>42*60+29</f>
+        <v>2549</v>
+      </c>
+      <c r="G33" s="6">
+        <f>40*60+34</f>
+        <v>2434</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J33" s="6">
+        <v>4</v>
+      </c>
+      <c r="K33" s="6">
+        <v>3</v>
+      </c>
+      <c r="L33" s="6">
+        <v>677.02</v>
+      </c>
+      <c r="M33" s="11">
+        <v>699.95</v>
+      </c>
+      <c r="N33" s="6">
+        <f>24*60+42</f>
+        <v>1482</v>
+      </c>
+      <c r="O33" s="6">
+        <f>25*60+42</f>
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" s="6">
+        <v>6</v>
+      </c>
+      <c r="C34" s="6">
+        <v>5</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1088.67</v>
+      </c>
+      <c r="E34" s="6">
+        <v>1115.21</v>
+      </c>
+      <c r="F34" s="6">
+        <f>41*60+46</f>
+        <v>2506</v>
+      </c>
+      <c r="G34" s="6">
+        <f>41*60+31</f>
+        <v>2491</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="6">
+        <v>4</v>
+      </c>
+      <c r="K34" s="6">
+        <v>3</v>
+      </c>
+      <c r="L34" s="6">
+        <v>787.09</v>
+      </c>
+      <c r="M34" s="11">
+        <v>676.83</v>
+      </c>
+      <c r="N34" s="6">
+        <f>28*60+20</f>
+        <v>1700</v>
+      </c>
+      <c r="O34" s="6">
+        <f>25*60+27</f>
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A35" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35" s="9">
+        <v>6</v>
+      </c>
+      <c r="C35" s="9">
+        <v>5</v>
+      </c>
+      <c r="D35" s="9">
+        <v>1130.9100000000001</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1164.46</v>
+      </c>
+      <c r="F35" s="9">
+        <f>43*60+5</f>
+        <v>2585</v>
+      </c>
+      <c r="G35" s="9">
+        <f>42*60+40</f>
+        <v>2560</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J35" s="9">
+        <v>4</v>
+      </c>
+      <c r="K35" s="9">
+        <v>3</v>
+      </c>
+      <c r="L35" s="9">
+        <v>761.41</v>
+      </c>
+      <c r="M35" s="9">
+        <v>678.32</v>
+      </c>
+      <c r="N35" s="9">
+        <f>27*60+38</f>
+        <v>1658</v>
+      </c>
+      <c r="O35" s="9">
+        <f>25*60+12</f>
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A36" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="I36" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="J36" s="27"/>
+      <c r="K36" s="27"/>
+      <c r="L36" s="27"/>
+      <c r="M36" s="27"/>
+      <c r="N36" s="27"/>
+      <c r="O36" s="27"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A37" s="6"/>
+      <c r="B37" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G37" s="27"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O37" s="27"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K38" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M38" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N38" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O38" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="6">
+        <v>7</v>
+      </c>
+      <c r="C39" s="6">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6">
+        <v>1357.26</v>
+      </c>
+      <c r="E39" s="11">
+        <v>1191.69</v>
+      </c>
+      <c r="F39" s="6">
+        <f>52*60+57</f>
+        <v>3177</v>
+      </c>
+      <c r="G39" s="6">
+        <f>48*60+9</f>
+        <v>2889</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="6">
+        <v>7</v>
+      </c>
+      <c r="K39" s="6">
+        <v>5</v>
+      </c>
+      <c r="L39" s="6">
+        <v>1596.1</v>
+      </c>
+      <c r="M39" s="11">
+        <v>1199.31</v>
+      </c>
+      <c r="N39" s="6">
+        <f>53*60+9</f>
+        <v>3189</v>
+      </c>
+      <c r="O39" s="6">
+        <f>43*60+14</f>
+        <v>2594</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="6">
+        <v>7</v>
+      </c>
+      <c r="C40" s="6">
+        <v>6</v>
+      </c>
+      <c r="D40" s="6">
+        <v>1243.5999999999999</v>
+      </c>
+      <c r="E40" s="11">
+        <v>1228.94</v>
+      </c>
+      <c r="F40" s="6">
+        <f>49*60+58</f>
+        <v>2998</v>
+      </c>
+      <c r="G40" s="6">
+        <f>48*60+51</f>
+        <v>2931</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J40" s="6">
+        <v>8</v>
+      </c>
+      <c r="K40" s="6">
+        <v>6</v>
+      </c>
+      <c r="L40" s="6">
+        <v>1720.39</v>
+      </c>
+      <c r="M40" s="11">
+        <v>1528</v>
+      </c>
+      <c r="N40" s="6">
+        <f>58*60+19</f>
+        <v>3499</v>
+      </c>
+      <c r="O40" s="6">
+        <f>51*60+29</f>
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" s="6">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6">
+        <v>6</v>
+      </c>
+      <c r="D41" s="6">
+        <v>1364.4</v>
+      </c>
+      <c r="E41" s="6">
+        <v>1281.9000000000001</v>
+      </c>
+      <c r="F41" s="6">
+        <f>51*60+32</f>
+        <v>3092</v>
+      </c>
+      <c r="G41" s="6">
+        <f>50*60+16</f>
+        <v>3016</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J41" s="6">
+        <v>7</v>
+      </c>
+      <c r="K41" s="6">
+        <v>5</v>
+      </c>
+      <c r="L41" s="6">
+        <v>1507.68</v>
+      </c>
+      <c r="M41" s="11">
+        <v>1251.02</v>
+      </c>
+      <c r="N41" s="6">
+        <f>52*60+38</f>
+        <v>3158</v>
+      </c>
+      <c r="O41" s="6">
+        <f>46*60+8</f>
+        <v>2768</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A42" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="9">
+        <v>7</v>
+      </c>
+      <c r="C42" s="9">
+        <v>5</v>
+      </c>
+      <c r="D42" s="9">
+        <v>1266.69</v>
+      </c>
+      <c r="E42" s="9">
+        <v>1053.68</v>
+      </c>
+      <c r="F42" s="9">
+        <f>49*60+57</f>
+        <v>2997</v>
+      </c>
+      <c r="G42" s="9">
+        <f>45*60+25</f>
+        <v>2725</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J42" s="9">
+        <v>8</v>
+      </c>
+      <c r="K42" s="9">
+        <v>5</v>
+      </c>
+      <c r="L42" s="9">
+        <v>1643.42</v>
+      </c>
+      <c r="M42" s="9">
+        <v>1245.5</v>
+      </c>
+      <c r="N42" s="9">
+        <f>56*60+26</f>
+        <v>3386</v>
+      </c>
+      <c r="O42" s="9">
+        <f>45*60+11</f>
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A43" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B43" s="27"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="I43" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="27"/>
+      <c r="M43" s="27"/>
+      <c r="N43" s="27"/>
+      <c r="O43" s="27"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A44" s="6"/>
+      <c r="B44" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E44" s="27"/>
+      <c r="F44" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G44" s="27"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M44" s="27"/>
+      <c r="N44" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O44" s="27"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K45" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M45" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O45" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="6">
+        <v>4</v>
+      </c>
+      <c r="C46" s="6">
+        <v>4</v>
+      </c>
+      <c r="D46" s="6">
+        <v>626.70000000000005</v>
+      </c>
+      <c r="E46" s="11">
+        <v>625.88</v>
+      </c>
+      <c r="F46" s="6">
+        <f>31*60+24</f>
+        <v>1884</v>
+      </c>
+      <c r="G46" s="6">
+        <f>30*60+56</f>
+        <v>1856</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="6">
+        <v>9</v>
+      </c>
+      <c r="K46" s="6">
+        <v>7</v>
+      </c>
+      <c r="L46" s="6">
+        <v>2027.64</v>
+      </c>
+      <c r="M46" s="11">
+        <v>1718.52</v>
+      </c>
+      <c r="N46" s="6">
+        <f>68*60+17</f>
+        <v>4097</v>
+      </c>
+      <c r="O46" s="6">
+        <f>61*60+32</f>
+        <v>3692</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="6">
+        <v>5</v>
+      </c>
+      <c r="C47" s="6">
+        <v>4</v>
+      </c>
+      <c r="D47" s="6">
+        <v>696.83</v>
+      </c>
+      <c r="E47" s="11">
+        <v>654.55999999999995</v>
+      </c>
+      <c r="F47" s="6">
+        <f>32*60+20</f>
+        <v>1940</v>
+      </c>
+      <c r="G47" s="6">
+        <f>31*60+25</f>
+        <v>1885</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J47" s="6">
+        <v>10</v>
+      </c>
+      <c r="K47" s="6">
+        <v>8</v>
+      </c>
+      <c r="L47" s="6">
+        <v>2128.67</v>
+      </c>
+      <c r="M47" s="11">
+        <v>1970.87</v>
+      </c>
+      <c r="N47" s="6">
+        <f>69*60+9</f>
+        <v>4149</v>
+      </c>
+      <c r="O47" s="6">
+        <f>67*60+0</f>
+        <v>4020</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B48" s="6">
+        <v>5</v>
+      </c>
+      <c r="C48" s="6">
+        <v>4</v>
+      </c>
+      <c r="D48" s="6">
+        <v>726.08</v>
+      </c>
+      <c r="E48" s="6">
+        <v>588.11</v>
+      </c>
+      <c r="F48" s="6">
+        <f>33*60+9</f>
+        <v>1989</v>
+      </c>
+      <c r="G48" s="6">
+        <f>30*60+1</f>
+        <v>1801</v>
+      </c>
+      <c r="I48" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J48" s="6">
+        <v>11</v>
+      </c>
+      <c r="K48" s="6">
+        <v>8</v>
+      </c>
+      <c r="L48" s="6">
+        <v>2426.3000000000002</v>
+      </c>
+      <c r="M48" s="6">
+        <f>1811.32</f>
+        <v>1811.32</v>
+      </c>
+      <c r="N48" s="6">
+        <f>76*60+43</f>
+        <v>4603</v>
+      </c>
+      <c r="O48" s="6">
+        <f>63*60+34</f>
+        <v>3814</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A49" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="9">
+        <v>5</v>
+      </c>
+      <c r="C49" s="9">
+        <v>4</v>
+      </c>
+      <c r="D49" s="9">
+        <v>715.55</v>
+      </c>
+      <c r="E49" s="9">
+        <v>713.51</v>
+      </c>
+      <c r="F49" s="9">
+        <f>33*60+25</f>
+        <v>2005</v>
+      </c>
+      <c r="G49" s="9">
+        <f>33*60+10</f>
+        <v>1990</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J49" s="9">
+        <v>10</v>
+      </c>
+      <c r="K49" s="9">
+        <v>7</v>
+      </c>
+      <c r="L49" s="9">
+        <v>2091.7800000000002</v>
+      </c>
+      <c r="M49" s="9">
+        <v>1748.65</v>
+      </c>
+      <c r="N49" s="9">
+        <f>68*60+47</f>
+        <v>4127</v>
+      </c>
+      <c r="O49" s="9">
+        <f>61*60+15</f>
+        <v>3675</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A50" s="28"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="6"/>
+      <c r="I50" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="27"/>
+      <c r="N50" s="27"/>
+      <c r="O50" s="27"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A51" s="6"/>
+      <c r="B51" s="27"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="27"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="27"/>
+      <c r="G51" s="27"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="K51" s="27"/>
+      <c r="L51" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="M51" s="27"/>
+      <c r="N51" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="O51" s="27"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6"/>
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="I53" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J53" s="6">
+        <v>5</v>
+      </c>
+      <c r="K53" s="6">
+        <v>4</v>
+      </c>
+      <c r="L53" s="6">
+        <v>832.25</v>
+      </c>
+      <c r="M53" s="11">
+        <v>807.44</v>
+      </c>
+      <c r="N53" s="6">
+        <f>38*60+13</f>
+        <v>2293</v>
+      </c>
+      <c r="O53" s="6">
+        <f>37*60+19</f>
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="I54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J54" s="6">
+        <v>5</v>
+      </c>
+      <c r="K54" s="6">
+        <v>4</v>
+      </c>
+      <c r="L54" s="6">
+        <v>770.17</v>
+      </c>
+      <c r="M54" s="11">
+        <v>785.78</v>
+      </c>
+      <c r="N54" s="6">
+        <f>36*60+54</f>
+        <v>2214</v>
+      </c>
+      <c r="O54" s="6">
+        <f>36*60+35</f>
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="I55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J55" s="6">
+        <v>6</v>
+      </c>
+      <c r="K55" s="6">
+        <v>4</v>
+      </c>
+      <c r="L55" s="6">
+        <v>848.18</v>
+      </c>
+      <c r="M55" s="11">
+        <v>800.63</v>
+      </c>
+      <c r="N55" s="6">
+        <f>37*60+37</f>
+        <v>2257</v>
+      </c>
+      <c r="O55" s="6">
+        <f>37*60+39</f>
+        <v>2259</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A56" s="9"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="I56" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J56" s="9">
+        <v>6</v>
+      </c>
+      <c r="K56" s="9">
+        <v>4</v>
+      </c>
+      <c r="L56" s="9">
+        <v>945.66</v>
+      </c>
+      <c r="M56" s="9">
+        <v>756.84</v>
+      </c>
+      <c r="N56" s="9">
+        <f>39*60+55</f>
+        <v>2395</v>
+      </c>
+      <c r="O56" s="9">
+        <f>36*60+22</f>
+        <v>2182</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="64">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A15:G15"/>
+    <mergeCell ref="A22:G22"/>
+    <mergeCell ref="A50:F50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="A43:G43"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I8:O8"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="A29:G29"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="I15:O15"/>
+    <mergeCell ref="I22:O22"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
+    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="I29:O29"/>
+    <mergeCell ref="I36:O36"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="N23:O23"/>
+    <mergeCell ref="I43:O43"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="L37:M37"/>
+    <mergeCell ref="N37:O37"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="N44:O44"/>
+    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="N51:O51"/>
+    <mergeCell ref="I50:O50"/>
+  </mergeCells>
+  <conditionalFormatting sqref="L32:L35">
+    <cfRule type="colorScale" priority="61">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M32:M35">
+    <cfRule type="colorScale" priority="60">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N32:N35">
+    <cfRule type="colorScale" priority="59">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O32:O35">
+    <cfRule type="colorScale" priority="58">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G4:G7">
+    <cfRule type="colorScale" priority="57">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4:F7">
+    <cfRule type="colorScale" priority="56">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:E7">
+    <cfRule type="colorScale" priority="55">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:D7">
+    <cfRule type="colorScale" priority="54">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11:L14">
+    <cfRule type="colorScale" priority="53">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M11:M14">
+    <cfRule type="colorScale" priority="52">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N11:N14">
+    <cfRule type="colorScale" priority="51">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O11:O14">
+    <cfRule type="colorScale" priority="50">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G18:G21">
+    <cfRule type="colorScale" priority="49">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18:F21">
+    <cfRule type="colorScale" priority="48">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18:E21">
+    <cfRule type="colorScale" priority="46">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D18:D21">
+    <cfRule type="colorScale" priority="45">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L18:L21">
+    <cfRule type="colorScale" priority="44">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M18:M21">
+    <cfRule type="colorScale" priority="43">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N18:N21">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O18:O21">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L53:L56">
+    <cfRule type="colorScale" priority="40">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M53:M56">
+    <cfRule type="colorScale" priority="39">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N53:N56">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O53:O56">
+    <cfRule type="colorScale" priority="37">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D25:D28">
+    <cfRule type="colorScale" priority="36">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25:E28">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F25:F28">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G25:G28">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L4:L7">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:M7">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N4:N7">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:O7">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L25:L28">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M25:M28">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N25:N28">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O25:O28">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L39:L42">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M39:M42">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N39:N42">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O39:O42">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L46:L49">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M46:M49">
+    <cfRule type="colorScale" priority="19">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N46:N49">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O46:O49">
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:D14">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E14">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11:F14">
+    <cfRule type="colorScale" priority="14">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G11:G14">
+    <cfRule type="colorScale" priority="13">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D32:D35">
+    <cfRule type="colorScale" priority="12">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32:E35">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F32:F35">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G32:G35">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D39:D42">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39:E42">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F39:F42">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G39:G42">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D46:D49">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46:E49">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F46:F49">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G46:G49">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>